<commit_message>
Pivot Table and deactivation one-hot encode in notebook 1
</commit_message>
<xml_diff>
--- a/data/profile_age_groups_import.xlsx
+++ b/data/profile_age_groups_import.xlsx
@@ -8,42 +8,58 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{6CABAFAB-52E6-492D-92B8-BB24B707BB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3928E498-9269-4EB7-BBC9-69A62D95EE05}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{CE9114DC-D55E-4DD2-8B05-AA322DEEF826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{566DF519-701A-4232-AC41-7E8C655A15E9}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="-120" windowWidth="36855" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profile_age_groups" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="8">
-  <si>
-    <t>18-35</t>
-  </si>
-  <si>
-    <t>36-45</t>
-  </si>
-  <si>
-    <t>46-55</t>
-  </si>
-  <si>
-    <t>56-65</t>
-  </si>
-  <si>
-    <t>66-75</t>
-  </si>
-  <si>
-    <t>76-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="9">
   <si>
     <t>age</t>
   </si>
   <si>
     <t>age_group</t>
+  </si>
+  <si>
+    <t>18-27</t>
+  </si>
+  <si>
+    <t>28-37</t>
+  </si>
+  <si>
+    <t>38-47</t>
+  </si>
+  <si>
+    <t>48-57</t>
+  </si>
+  <si>
+    <t>58-67</t>
+  </si>
+  <si>
+    <t>68-77</t>
+  </si>
+  <si>
+    <t>78-</t>
   </si>
 </sst>
 </file>
@@ -870,17 +886,17 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B62" sqref="B62:B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -888,7 +904,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -896,7 +912,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -904,7 +920,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -912,7 +928,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -920,7 +936,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -928,7 +944,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -936,7 +952,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -944,7 +960,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -952,7 +968,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -960,7 +976,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -968,7 +984,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -976,7 +992,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -984,7 +1000,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -992,7 +1008,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -1000,7 +1016,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -1008,7 +1024,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -1016,7 +1032,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -1024,7 +1040,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -1032,7 +1048,7 @@
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -1040,7 +1056,7 @@
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -1048,7 +1064,7 @@
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -1056,7 +1072,7 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -1064,7 +1080,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -1072,7 +1088,7 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -1080,7 +1096,7 @@
         <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -1088,7 +1104,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -1096,7 +1112,7 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -1104,7 +1120,7 @@
         <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -1112,7 +1128,7 @@
         <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -1120,7 +1136,7 @@
         <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -1128,7 +1144,7 @@
         <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -1136,7 +1152,7 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -1144,7 +1160,7 @@
         <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -1152,7 +1168,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -1160,7 +1176,7 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -1168,7 +1184,7 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -1176,7 +1192,7 @@
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -1184,7 +1200,7 @@
         <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -1192,7 +1208,7 @@
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -1200,7 +1216,7 @@
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -1208,7 +1224,7 @@
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -1216,7 +1232,7 @@
         <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -1224,7 +1240,7 @@
         <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -1232,7 +1248,7 @@
         <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -1240,7 +1256,7 @@
         <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -1248,7 +1264,7 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -1256,7 +1272,7 @@
         <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -1264,7 +1280,7 @@
         <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -1272,7 +1288,7 @@
         <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -1280,7 +1296,7 @@
         <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -1288,7 +1304,7 @@
         <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -1296,7 +1312,7 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -1304,7 +1320,7 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -1312,7 +1328,7 @@
         <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -1320,7 +1336,7 @@
         <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -1328,7 +1344,7 @@
         <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -1336,7 +1352,7 @@
         <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -1344,7 +1360,7 @@
         <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -1352,7 +1368,7 @@
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -1360,7 +1376,7 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -1368,7 +1384,7 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -1376,7 +1392,7 @@
         <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -1384,7 +1400,7 @@
         <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -1392,7 +1408,7 @@
         <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -1400,7 +1416,7 @@
         <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -1408,7 +1424,7 @@
         <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -1416,7 +1432,7 @@
         <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -1424,7 +1440,7 @@
         <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -1432,7 +1448,7 @@
         <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
@@ -1440,7 +1456,7 @@
         <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
@@ -1448,7 +1464,7 @@
         <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
@@ -1456,7 +1472,7 @@
         <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.4">
@@ -1464,7 +1480,7 @@
         <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.4">
@@ -1472,7 +1488,7 @@
         <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
@@ -1480,7 +1496,7 @@
         <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.4">
@@ -1488,7 +1504,7 @@
         <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.4">
@@ -1496,7 +1512,7 @@
         <v>94</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
@@ -1504,7 +1520,7 @@
         <v>95</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.4">
@@ -1512,7 +1528,7 @@
         <v>96</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.4">
@@ -1520,7 +1536,7 @@
         <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.4">
@@ -1528,7 +1544,7 @@
         <v>98</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.4">
@@ -1536,7 +1552,7 @@
         <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.4">
@@ -1544,7 +1560,7 @@
         <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.4">
@@ -1552,7 +1568,7 @@
         <v>101</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.4">
@@ -1560,7 +1576,7 @@
         <v>102</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.4">
@@ -1568,7 +1584,7 @@
         <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.4">
@@ -1576,7 +1592,7 @@
         <v>104</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.4">
@@ -1584,7 +1600,7 @@
         <v>105</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.4">
@@ -1592,7 +1608,7 @@
         <v>106</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.4">
@@ -1600,7 +1616,7 @@
         <v>107</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.4">
@@ -1608,7 +1624,7 @@
         <v>108</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.4">
@@ -1616,7 +1632,7 @@
         <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.4">
@@ -1624,7 +1640,7 @@
         <v>110</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.4">
@@ -1632,7 +1648,7 @@
         <v>111</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.4">
@@ -1640,7 +1656,7 @@
         <v>112</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.4">
@@ -1648,7 +1664,7 @@
         <v>113</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.4">
@@ -1656,7 +1672,7 @@
         <v>114</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.4">
@@ -1664,7 +1680,7 @@
         <v>115</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>